<commit_message>
Mainboard: update BOM, fabrication print
</commit_message>
<xml_diff>
--- a/hardware/mainboard/mainboard-BOM.xlsx
+++ b/hardware/mainboard/mainboard-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Desktop\tmp\mainboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\yozh\hardware\mainboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550BA64E-5CB5-44B8-A7D8-B635F5CDFF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7437BE-CBF7-40F2-8283-B9F39CA8B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="17510" windowHeight="9550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2650" yWindow="300" windowWidth="15120" windowHeight="9550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mainboard_bom_" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="144">
   <si>
     <t>Component</t>
   </si>
@@ -211,9 +211,6 @@
     <t>USB_Micro-B_Amphenol_10118194_Horizontal</t>
   </si>
   <si>
-    <t>C145779</t>
-  </si>
-  <si>
     <t>R1 R9 R10</t>
   </si>
   <si>
@@ -443,6 +440,18 @@
   </si>
   <si>
     <t>Male header, 2*4p, 0.1"</t>
+  </si>
+  <si>
+    <t>C132563</t>
+  </si>
+  <si>
+    <t>C92271</t>
+  </si>
+  <si>
+    <t>C92269</t>
+  </si>
+  <si>
+    <t>C52711</t>
   </si>
 </sst>
 </file>
@@ -1288,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1311,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1326,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
@@ -1335,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1343,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1358,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
@@ -1372,10 +1381,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -1387,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -1401,10 +1410,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -1416,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -1430,7 +1439,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1445,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -1459,7 +1468,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1474,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" t="s">
         <v>11</v>
@@ -1488,7 +1497,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -1503,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
@@ -1517,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -1532,13 +1541,13 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -1546,7 +1555,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
@@ -1564,13 +1573,13 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -1578,7 +1587,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -1596,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" t="s">
         <v>37</v>
@@ -1625,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>
@@ -1642,7 +1651,7 @@
         <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
@@ -1654,13 +1663,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I12" t="s">
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1668,28 +1677,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>66</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1697,28 +1706,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
         <v>68</v>
       </c>
-      <c r="E14" t="s">
-        <v>69</v>
-      </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" t="s">
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1726,28 +1735,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" t="s">
-        <v>72</v>
-      </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15">
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1755,28 +1764,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" t="s">
         <v>74</v>
-      </c>
-      <c r="F16" t="s">
-        <v>75</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I16" t="s">
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1784,28 +1793,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
         <v>116</v>
       </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
       <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" t="s">
         <v>76</v>
-      </c>
-      <c r="F17" t="s">
-        <v>77</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17" t="s">
         <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1813,31 +1822,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="C18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" t="s">
         <v>79</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" t="s">
-        <v>80</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1845,31 +1854,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
         <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" t="s">
-        <v>85</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" t="s">
         <v>86</v>
-      </c>
-      <c r="J19" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1877,31 +1886,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>89</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
         <v>90</v>
-      </c>
-      <c r="E20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" t="s">
-        <v>91</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I20" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" t="s">
         <v>92</v>
-      </c>
-      <c r="J20" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -1909,28 +1918,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" t="s">
         <v>94</v>
       </c>
-      <c r="C21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>96</v>
-      </c>
-      <c r="E21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" t="s">
-        <v>97</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -1941,7 +1950,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
@@ -1953,13 +1962,13 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
       </c>
       <c r="J22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -1967,7 +1976,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
@@ -1979,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
@@ -1990,19 +1999,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
@@ -2013,7 +2022,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
@@ -2025,7 +2034,7 @@
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
@@ -2036,7 +2045,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
         <v>50</v>
@@ -2048,7 +2057,7 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
@@ -2059,7 +2068,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
         <v>52</v>
@@ -2071,10 +2080,13 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2082,7 +2094,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
@@ -2094,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -2105,7 +2117,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" t="s">
         <v>56</v>
@@ -2117,10 +2129,13 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I29" t="s">
         <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2128,7 +2143,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
         <v>58</v>
@@ -2140,10 +2155,13 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>